<commit_message>
Addition of staging work
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/CustomOrder/QA_537.xlsx
+++ b/testdata/FCfiles/qa/CustomOrder/QA_537.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="127">
   <si>
     <t>shipmentType</t>
   </si>
@@ -404,6 +404,9 @@
   </si>
   <si>
     <t>51527537</t>
+  </si>
+  <si>
+    <t>51528291</t>
   </si>
 </sst>
 </file>
@@ -440,7 +443,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="44">
+  <fills count="48">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -657,8 +660,28 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="45">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -875,12 +898,26 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -918,7 +955,9 @@
     <xf applyBorder="true" applyFill="true" borderId="38" fillId="37" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="40" fillId="39" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="42" fillId="41" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="44" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="44" fillId="43" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="46" fillId="45" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="48" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1603,8 +1642,8 @@
       <c r="T5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U5" s="37" t="s">
-        <v>125</v>
+      <c r="U5" s="39" t="s">
+        <v>126</v>
       </c>
       <c r="V5" s="14" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Username change for overage
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/CustomOrder/QA_537.xlsx
+++ b/testdata/FCfiles/qa/CustomOrder/QA_537.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="128">
   <si>
     <t>shipmentType</t>
   </si>
@@ -407,6 +407,9 @@
   </si>
   <si>
     <t>51528291</t>
+  </si>
+  <si>
+    <t>51532616</t>
   </si>
 </sst>
 </file>
@@ -443,7 +446,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="48">
+  <fills count="52">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -680,8 +683,28 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="49">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -912,12 +935,26 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -957,7 +994,9 @@
     <xf applyBorder="true" applyFill="true" borderId="42" fillId="41" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="44" fillId="43" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="46" fillId="45" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="48" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="48" fillId="47" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="50" fillId="49" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="51" borderId="52" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1642,8 +1681,8 @@
       <c r="T5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U5" s="39" t="s">
-        <v>126</v>
+      <c r="U5" s="41" t="s">
+        <v>127</v>
       </c>
       <c r="V5" s="14" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Request reroute update in xml file.
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/CustomOrder/QA_537.xlsx
+++ b/testdata/FCfiles/qa/CustomOrder/QA_537.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="129">
   <si>
     <t>shipmentType</t>
   </si>
@@ -410,6 +410,9 @@
   </si>
   <si>
     <t>51532616</t>
+  </si>
+  <si>
+    <t>51538948</t>
   </si>
 </sst>
 </file>
@@ -446,7 +449,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="52">
+  <fills count="56">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -703,8 +706,28 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="53">
+  <borders count="57">
     <border>
       <left/>
       <right/>
@@ -949,12 +972,26 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -996,7 +1033,9 @@
     <xf applyBorder="true" applyFill="true" borderId="46" fillId="45" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="48" fillId="47" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="50" fillId="49" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="51" borderId="52" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="52" fillId="51" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="54" fillId="53" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="55" borderId="56" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1681,8 +1720,8 @@
       <c r="T5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U5" s="41" t="s">
-        <v>127</v>
+      <c r="U5" s="43" t="s">
+        <v>128</v>
       </c>
       <c r="V5" s="14" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Updated email notification for custom order and reroute
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/CustomOrder/QA_537.xlsx
+++ b/testdata/FCfiles/qa/CustomOrder/QA_537.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="130">
   <si>
     <t>shipmentType</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t>51538948</t>
+  </si>
+  <si>
+    <t>51539140</t>
   </si>
 </sst>
 </file>
@@ -449,7 +452,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="56">
+  <fills count="60">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -726,8 +729,28 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="57">
+  <borders count="61">
     <border>
       <left/>
       <right/>
@@ -986,12 +1009,26 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -1035,7 +1072,9 @@
     <xf applyBorder="true" applyFill="true" borderId="50" fillId="49" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="52" fillId="51" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="54" fillId="53" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="55" borderId="56" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="56" fillId="55" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="58" fillId="57" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="59" borderId="60" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1720,8 +1759,8 @@
       <c r="T5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U5" s="43" t="s">
-        <v>128</v>
+      <c r="U5" s="45" t="s">
+        <v>129</v>
       </c>
       <c r="V5" s="14" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Drop off location name issue fixed
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/CustomOrder/QA_537.xlsx
+++ b/testdata/FCfiles/qa/CustomOrder/QA_537.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="133">
   <si>
     <t>shipmentType</t>
   </si>
@@ -422,6 +422,9 @@
   </si>
   <si>
     <t>51540114</t>
+  </si>
+  <si>
+    <t>51542047</t>
   </si>
 </sst>
 </file>
@@ -458,7 +461,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="68">
+  <fills count="72">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -795,8 +798,28 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="69">
+  <borders count="73">
     <border>
       <left/>
       <right/>
@@ -1097,12 +1120,26 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -1152,7 +1189,9 @@
     <xf applyBorder="true" applyFill="true" borderId="62" fillId="61" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="64" fillId="63" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="66" fillId="65" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="67" borderId="68" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="68" fillId="67" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="70" fillId="69" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="71" borderId="72" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1837,8 +1876,8 @@
       <c r="T5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U5" s="49" t="s">
-        <v>131</v>
+      <c r="U5" s="51" t="s">
+        <v>132</v>
       </c>
       <c r="V5" s="14" t="s">
         <v>99</v>

</xml_diff>

<commit_message>
Manage billing and xml update regarding delivery checkbox in manage carrier
</commit_message>
<xml_diff>
--- a/testdata/FCfiles/qa/CustomOrder/QA_537.xlsx
+++ b/testdata/FCfiles/qa/CustomOrder/QA_537.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="134">
   <si>
     <t>shipmentType</t>
   </si>
@@ -425,6 +425,9 @@
   </si>
   <si>
     <t>51542047</t>
+  </si>
+  <si>
+    <t>51545893</t>
   </si>
 </sst>
 </file>
@@ -461,7 +464,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="72">
+  <fills count="76">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -818,8 +821,28 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="73">
+  <borders count="77">
     <border>
       <left/>
       <right/>
@@ -1134,12 +1157,26 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
@@ -1191,7 +1228,9 @@
     <xf applyBorder="true" applyFill="true" borderId="66" fillId="65" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="68" fillId="67" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="70" fillId="69" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="71" borderId="72" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="72" fillId="71" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="74" fillId="73" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="75" borderId="76" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1876,8 +1915,8 @@
       <c r="T5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="U5" s="51" t="s">
-        <v>132</v>
+      <c r="U5" s="53" t="s">
+        <v>133</v>
       </c>
       <c r="V5" s="14" t="s">
         <v>99</v>

</xml_diff>